<commit_message>
added TSP solutions acquired with solver
</commit_message>
<xml_diff>
--- a/TSP/Dane_TSP_76.xlsx
+++ b/TSP/Dane_TSP_76.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\Programowanie\ComputationalInteligence\TSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3186C4F8-6BED-4B0E-88DF-5D5F7A87784A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E0E48A-BD53-4576-83BE-03329AD797F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2E92C40E-D2D6-4D6C-8826-671A9922C679}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{2E92C40E-D2D6-4D6C-8826-671A9922C679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -383,11 +383,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA78BEE2-21FA-481B-9D61-3C52918C26C9}">
   <dimension ref="A1:BY77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -617,10 +619,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
         <v>1118.0339887498949</v>
       </c>
@@ -847,13 +852,16 @@
         <v>3716.180835212409</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1118.0339887498949</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
       <c r="D3">
         <v>2926.1749776799061</v>
       </c>
@@ -1077,7 +1085,7 @@
         <v>3828.8379438153288</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1087,6 +1095,9 @@
       <c r="C4">
         <v>2926.1749776799061</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4">
         <v>700</v>
       </c>
@@ -1307,7 +1318,7 @@
         <v>6689.7309362933274</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1320,6 +1331,9 @@
       <c r="D5">
         <v>700</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <v>1368.89480969138</v>
       </c>
@@ -1537,7 +1551,7 @@
         <v>7179.3105518566344</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1553,6 +1567,9 @@
       <c r="E6">
         <v>1368.89480969138</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
       <c r="G6">
         <v>1115.0004484304029</v>
       </c>
@@ -1767,7 +1784,7 @@
         <v>8305.0751351206927</v>
       </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1786,6 +1803,9 @@
       <c r="F7">
         <v>1115.0004484304029</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
       <c r="H7">
         <v>905.84380552057644</v>
       </c>
@@ -1997,7 +2017,7 @@
         <v>7625.2903551274694</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2019,6 +2039,9 @@
       <c r="G8">
         <v>905.84380552057644</v>
       </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8">
         <v>583.09518948453001</v>
       </c>
@@ -2227,7 +2250,7 @@
         <v>7027.2683170631817</v>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2252,6 +2275,9 @@
       <c r="H9">
         <v>583.09518948453001</v>
       </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
       <c r="J9">
         <v>2000</v>
       </c>
@@ -2457,7 +2483,7 @@
         <v>7071.9516401061464</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2485,6 +2511,9 @@
       <c r="I10">
         <v>2000</v>
       </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
       <c r="K10">
         <v>700</v>
       </c>
@@ -2687,7 +2716,7 @@
         <v>8875.3873154922094</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2718,6 +2747,9 @@
       <c r="J11">
         <v>700</v>
       </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
       <c r="L11">
         <v>1616.696941297286</v>
       </c>
@@ -2917,7 +2949,7 @@
         <v>9250</v>
       </c>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2951,6 +2983,9 @@
       <c r="K12">
         <v>1616.696941297286</v>
       </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
       <c r="M12">
         <v>1118.0004472271021</v>
       </c>
@@ -3147,7 +3182,7 @@
         <v>10718.49378410978</v>
       </c>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3184,6 +3219,9 @@
       <c r="L13">
         <v>1118.0004472271021</v>
       </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="N13">
         <v>1164.11683262463</v>
       </c>
@@ -3377,7 +3415,7 @@
         <v>10199.057211330861</v>
       </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3417,6 +3455,9 @@
       <c r="M14">
         <v>1164.11683262463</v>
       </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
       <c r="O14">
         <v>522.01532544552754</v>
       </c>
@@ -3607,7 +3648,7 @@
         <v>10562.196741208711</v>
       </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3650,6 +3691,9 @@
       <c r="N15">
         <v>522.01532544552754</v>
       </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
       <c r="P15">
         <v>1746.424919657298</v>
       </c>
@@ -3837,7 +3881,7 @@
         <v>10556.15933945675</v>
       </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3883,6 +3927,9 @@
       <c r="O16">
         <v>1746.424919657298</v>
       </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
       <c r="Q16">
         <v>700</v>
       </c>
@@ -4067,7 +4114,7 @@
         <v>11746.169588423279</v>
       </c>
     </row>
-    <row r="17" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4116,6 +4163,9 @@
       <c r="P17">
         <v>700</v>
       </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
       <c r="R17">
         <v>1511.6216457830969</v>
       </c>
@@ -4297,7 +4347,7 @@
         <v>12031.728886573201</v>
       </c>
     </row>
-    <row r="18" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4349,6 +4399,9 @@
       <c r="Q18">
         <v>1511.6216457830969</v>
       </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
       <c r="S18">
         <v>667.08320320631674</v>
       </c>
@@ -4527,7 +4580,7 @@
         <v>11899.684869777009</v>
       </c>
     </row>
-    <row r="19" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4582,6 +4635,9 @@
       <c r="R19">
         <v>667.08320320631674</v>
       </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
       <c r="T19">
         <v>3700</v>
       </c>
@@ -4757,7 +4813,7 @@
         <v>12386.787315522941</v>
       </c>
     </row>
-    <row r="20" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4815,6 +4871,9 @@
       <c r="S20">
         <v>3700</v>
       </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
       <c r="U20">
         <v>715.89105316381767</v>
       </c>
@@ -4987,7 +5046,7 @@
         <v>9592.3146320374617</v>
       </c>
     </row>
-    <row r="21" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5048,6 +5107,9 @@
       <c r="T21">
         <v>715.89105316381767</v>
       </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
       <c r="V21">
         <v>3707.4249823833252</v>
       </c>
@@ -5217,7 +5279,7 @@
         <v>8912.0704665077683</v>
       </c>
     </row>
-    <row r="22" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5281,6 +5343,9 @@
       <c r="U22">
         <v>3707.4249823833252</v>
       </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
       <c r="W22">
         <v>1192.6860441876561</v>
       </c>
@@ -5447,7 +5512,7 @@
         <v>7527.2837066235252</v>
       </c>
     </row>
-    <row r="23" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5514,6 +5579,9 @@
       <c r="V23">
         <v>1192.6860441876561</v>
       </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
       <c r="X23">
         <v>1432.6548781894401</v>
       </c>
@@ -5677,7 +5745,7 @@
         <v>6622.1220163932348</v>
       </c>
     </row>
-    <row r="24" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5747,6 +5815,9 @@
       <c r="W24">
         <v>1432.6548781894401</v>
       </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
       <c r="Y24">
         <v>3031.913587159107</v>
       </c>
@@ -5907,7 +5978,7 @@
         <v>5261.1785751863617</v>
       </c>
     </row>
-    <row r="25" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5980,6 +6051,9 @@
       <c r="X25">
         <v>3031.913587159107</v>
       </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
       <c r="Z25">
         <v>1118.0339887498949</v>
       </c>
@@ -6137,7 +6211,7 @@
         <v>8286.8872322483057</v>
       </c>
     </row>
-    <row r="26" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6213,6 +6287,9 @@
       <c r="Y26">
         <v>1118.0339887498949</v>
       </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
       <c r="AA26">
         <v>2926.1749776799061</v>
       </c>
@@ -6367,7 +6444,7 @@
         <v>8048.1364302551428</v>
       </c>
     </row>
-    <row r="27" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6446,6 +6523,9 @@
       <c r="Z27">
         <v>2926.1749776799061</v>
       </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
       <c r="AB27">
         <v>700</v>
       </c>
@@ -6597,7 +6677,7 @@
         <v>10491.186777481371</v>
       </c>
     </row>
-    <row r="28" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6679,6 +6759,9 @@
       <c r="AA28">
         <v>700</v>
       </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
       <c r="AC28">
         <v>1368.89480969138</v>
       </c>
@@ -6827,7 +6910,7 @@
         <v>11113.28034380488</v>
       </c>
     </row>
-    <row r="29" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6912,6 +6995,9 @@
       <c r="AB29">
         <v>1368.89480969138</v>
       </c>
+      <c r="AC29">
+        <v>0</v>
+      </c>
       <c r="AD29">
         <v>1115.0004484304029</v>
       </c>
@@ -7057,7 +7143,7 @@
         <v>11954.613042671021</v>
       </c>
     </row>
-    <row r="30" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -7145,6 +7231,9 @@
       <c r="AC30">
         <v>1115.0004484304029</v>
       </c>
+      <c r="AD30">
+        <v>0</v>
+      </c>
       <c r="AE30">
         <v>905.84380552057644</v>
       </c>
@@ -7287,7 +7376,7 @@
         <v>11022.297990891009</v>
       </c>
     </row>
-    <row r="31" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -7378,6 +7467,9 @@
       <c r="AD31">
         <v>905.84380552057644</v>
       </c>
+      <c r="AE31">
+        <v>0</v>
+      </c>
       <c r="AF31">
         <v>583.09518948453001</v>
       </c>
@@ -7517,7 +7609,7 @@
         <v>10210.0440743417</v>
       </c>
     </row>
-    <row r="32" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -7611,6 +7703,9 @@
       <c r="AE32">
         <v>583.09518948453001</v>
       </c>
+      <c r="AF32">
+        <v>0</v>
+      </c>
       <c r="AG32">
         <v>2000</v>
       </c>
@@ -7747,7 +7842,7 @@
         <v>10006.248048094751</v>
       </c>
     </row>
-    <row r="33" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -7844,6 +7939,9 @@
       <c r="AF33">
         <v>2000</v>
       </c>
+      <c r="AG33">
+        <v>0</v>
+      </c>
       <c r="AH33">
         <v>700</v>
       </c>
@@ -7977,7 +8075,7 @@
         <v>12003.54114417908</v>
       </c>
     </row>
-    <row r="34" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -8077,6 +8175,9 @@
       <c r="AG34">
         <v>700</v>
       </c>
+      <c r="AH34">
+        <v>0</v>
+      </c>
       <c r="AI34">
         <v>1616.696941297286</v>
       </c>
@@ -8207,7 +8308,7 @@
         <v>12550.896382330629</v>
       </c>
     </row>
-    <row r="35" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -8310,6 +8411,9 @@
       <c r="AH35">
         <v>1616.696941297286</v>
       </c>
+      <c r="AI35">
+        <v>0</v>
+      </c>
       <c r="AJ35">
         <v>1118.0004472271021</v>
       </c>
@@ -8437,7 +8541,7 @@
         <v>13742.038022069361</v>
       </c>
     </row>
-    <row r="36" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -8543,6 +8647,9 @@
       <c r="AI36">
         <v>1118.0004472271021</v>
       </c>
+      <c r="AJ36">
+        <v>0</v>
+      </c>
       <c r="AK36">
         <v>1164.11683262463</v>
       </c>
@@ -8667,7 +8774,7 @@
         <v>12936.663712101359</v>
       </c>
     </row>
-    <row r="37" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -8776,6 +8883,9 @@
       <c r="AJ37">
         <v>1164.11683262463</v>
       </c>
+      <c r="AK37">
+        <v>0</v>
+      </c>
       <c r="AL37">
         <v>522.01532544552754</v>
       </c>
@@ -8897,7 +9007,7 @@
         <v>12900.48448702606</v>
       </c>
     </row>
-    <row r="38" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -9009,6 +9119,9 @@
       <c r="AK38">
         <v>522.01532544552754</v>
       </c>
+      <c r="AL38">
+        <v>0</v>
+      </c>
       <c r="AM38">
         <v>1746.424919657298</v>
       </c>
@@ -9127,7 +9240,7 @@
         <v>12710.03540514345</v>
       </c>
     </row>
-    <row r="39" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -9242,6 +9355,9 @@
       <c r="AL39">
         <v>1746.424919657298</v>
       </c>
+      <c r="AM39">
+        <v>0</v>
+      </c>
       <c r="AN39">
         <v>700</v>
       </c>
@@ -9357,7 +9473,7 @@
         <v>14257.804880134951</v>
       </c>
     </row>
-    <row r="40" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -9475,6 +9591,9 @@
       <c r="AM40">
         <v>700</v>
       </c>
+      <c r="AN40">
+        <v>0</v>
+      </c>
       <c r="AO40">
         <v>1511.6216457830969</v>
       </c>
@@ -9587,7 +9706,7 @@
         <v>14721.58279533828</v>
       </c>
     </row>
-    <row r="41" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -9708,6 +9827,9 @@
       <c r="AN41">
         <v>1511.6216457830969</v>
       </c>
+      <c r="AO41">
+        <v>0</v>
+      </c>
       <c r="AP41">
         <v>667.08320320631674</v>
       </c>
@@ -9817,7 +9939,7 @@
         <v>15014.65950329877</v>
       </c>
     </row>
-    <row r="42" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -9941,6 +10063,9 @@
       <c r="AO42">
         <v>667.08320320631674</v>
       </c>
+      <c r="AP42">
+        <v>0</v>
+      </c>
       <c r="AQ42">
         <v>3700</v>
       </c>
@@ -10047,7 +10172,7 @@
         <v>15602.72412112705</v>
       </c>
     </row>
-    <row r="43" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10174,6 +10299,9 @@
       <c r="AP43">
         <v>3700</v>
       </c>
+      <c r="AQ43">
+        <v>0</v>
+      </c>
       <c r="AR43">
         <v>715.89105316381767</v>
       </c>
@@ -10277,7 +10405,7 @@
         <v>13491.664093061319</v>
       </c>
     </row>
-    <row r="44" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -10407,6 +10535,9 @@
       <c r="AQ44">
         <v>715.89105316381767</v>
       </c>
+      <c r="AR44">
+        <v>0</v>
+      </c>
       <c r="AS44">
         <v>3707.4249823833252</v>
       </c>
@@ -10507,7 +10638,7 @@
         <v>12777.421492617361</v>
       </c>
     </row>
-    <row r="45" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -10640,6 +10771,9 @@
       <c r="AR45">
         <v>3707.4249823833252</v>
       </c>
+      <c r="AS45">
+        <v>0</v>
+      </c>
       <c r="AT45">
         <v>1192.6860441876561</v>
       </c>
@@ -10737,7 +10871,7 @@
         <v>12110.842249818959</v>
       </c>
     </row>
-    <row r="46" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -10873,6 +11007,9 @@
       <c r="AS46">
         <v>1192.6860441876561</v>
       </c>
+      <c r="AT46">
+        <v>0</v>
+      </c>
       <c r="AU46">
         <v>1432.6548781894401</v>
       </c>
@@ -10967,7 +11104,7 @@
         <v>11300</v>
       </c>
     </row>
-    <row r="47" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11106,6 +11243,9 @@
       <c r="AT47">
         <v>1432.6548781894401</v>
       </c>
+      <c r="AU47">
+        <v>0</v>
+      </c>
       <c r="AV47">
         <v>3031.913587159107</v>
       </c>
@@ -11197,7 +11337,7 @@
         <v>9982.1089955980751</v>
       </c>
     </row>
-    <row r="48" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11339,6 +11479,9 @@
       <c r="AU48">
         <v>3031.913587159107</v>
       </c>
+      <c r="AV48">
+        <v>0</v>
+      </c>
       <c r="AW48">
         <v>1118.0339887498949</v>
       </c>
@@ -11427,7 +11570,7 @@
         <v>12986.916493148021</v>
       </c>
     </row>
-    <row r="49" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11572,6 +11715,9 @@
       <c r="AV49">
         <v>1118.0339887498949</v>
       </c>
+      <c r="AW49">
+        <v>0</v>
+      </c>
       <c r="AX49">
         <v>2926.1749776799061</v>
       </c>
@@ -11657,7 +11803,7 @@
         <v>12649.50591920491</v>
       </c>
     </row>
-    <row r="50" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -11805,6 +11951,9 @@
       <c r="AW50">
         <v>2926.1749776799061</v>
       </c>
+      <c r="AX50">
+        <v>0</v>
+      </c>
       <c r="AY50">
         <v>700</v>
       </c>
@@ -11887,7 +12036,7 @@
         <v>14849.32658405761</v>
       </c>
     </row>
-    <row r="51" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -12038,6 +12187,9 @@
       <c r="AX51">
         <v>700</v>
       </c>
+      <c r="AY51">
+        <v>0</v>
+      </c>
       <c r="AZ51">
         <v>1368.89480969138</v>
       </c>
@@ -12117,7 +12269,7 @@
         <v>15511.044452260459</v>
       </c>
     </row>
-    <row r="52" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -12271,6 +12423,9 @@
       <c r="AY52">
         <v>1368.89480969138</v>
       </c>
+      <c r="AZ52">
+        <v>0</v>
+      </c>
       <c r="BA52">
         <v>1115.0004484304029</v>
       </c>
@@ -12347,7 +12502,7 @@
         <v>16185.681110166481</v>
       </c>
     </row>
-    <row r="53" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -12504,6 +12659,9 @@
       <c r="AZ53">
         <v>1115.0004484304029</v>
       </c>
+      <c r="BA53">
+        <v>0</v>
+      </c>
       <c r="BB53">
         <v>905.84380552057644</v>
       </c>
@@ -12577,7 +12735,7 @@
         <v>15164.499760954861</v>
       </c>
     </row>
-    <row r="54" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -12737,6 +12895,9 @@
       <c r="BA54">
         <v>905.84380552057644</v>
       </c>
+      <c r="BB54">
+        <v>0</v>
+      </c>
       <c r="BC54">
         <v>583.09518948453001</v>
       </c>
@@ -12807,7 +12968,7 @@
         <v>14290.99366734168</v>
       </c>
     </row>
-    <row r="55" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -12970,6 +13131,9 @@
       <c r="BB55">
         <v>583.09518948453001</v>
       </c>
+      <c r="BC55">
+        <v>0</v>
+      </c>
       <c r="BD55">
         <v>2000</v>
       </c>
@@ -13037,7 +13201,7 @@
         <v>13977.213599283659</v>
       </c>
     </row>
-    <row r="56" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -13203,6 +13367,9 @@
       <c r="BC56">
         <v>2000</v>
       </c>
+      <c r="BD56">
+        <v>0</v>
+      </c>
       <c r="BE56">
         <v>700</v>
       </c>
@@ -13267,7 +13434,7 @@
         <v>15953.7613119916</v>
       </c>
     </row>
-    <row r="57" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -13436,6 +13603,9 @@
       <c r="BD57">
         <v>700</v>
       </c>
+      <c r="BE57">
+        <v>0</v>
+      </c>
       <c r="BF57">
         <v>1616.696941297286</v>
       </c>
@@ -13497,7 +13667,7 @@
         <v>16571.43626847112</v>
       </c>
     </row>
-    <row r="58" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -13669,6 +13839,9 @@
       <c r="BE58">
         <v>1616.696941297286</v>
       </c>
+      <c r="BF58">
+        <v>0</v>
+      </c>
       <c r="BG58">
         <v>1118.0004472271021</v>
       </c>
@@ -13727,7 +13900,7 @@
         <v>17547.823483269942</v>
       </c>
     </row>
-    <row r="59" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -13902,6 +14075,9 @@
       <c r="BF59">
         <v>1118.0004472271021</v>
       </c>
+      <c r="BG59">
+        <v>0</v>
+      </c>
       <c r="BH59">
         <v>1164.11683262463</v>
       </c>
@@ -13957,7 +14133,7 @@
         <v>16607.79238791237</v>
       </c>
     </row>
-    <row r="60" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -14135,6 +14311,9 @@
       <c r="BG60">
         <v>1164.11683262463</v>
       </c>
+      <c r="BH60">
+        <v>0</v>
+      </c>
       <c r="BI60">
         <v>522.01532544552754</v>
       </c>
@@ -14187,7 +14366,7 @@
         <v>16322.07094703365</v>
       </c>
     </row>
-    <row r="61" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -14368,6 +14547,9 @@
       <c r="BH61">
         <v>522.01532544552754</v>
       </c>
+      <c r="BI61">
+        <v>0</v>
+      </c>
       <c r="BJ61">
         <v>1746.424919657298</v>
       </c>
@@ -14417,7 +14599,7 @@
         <v>16024.434467400089</v>
       </c>
     </row>
-    <row r="62" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -14601,6 +14783,9 @@
       <c r="BI62">
         <v>1746.424919657298</v>
       </c>
+      <c r="BJ62">
+        <v>0</v>
+      </c>
       <c r="BK62">
         <v>700</v>
       </c>
@@ -14647,7 +14832,7 @@
         <v>17712.213300431991</v>
       </c>
     </row>
-    <row r="63" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -14834,6 +15019,9 @@
       <c r="BJ63">
         <v>700</v>
       </c>
+      <c r="BK63">
+        <v>0</v>
+      </c>
       <c r="BL63">
         <v>1511.6216457830969</v>
       </c>
@@ -14877,7 +15065,7 @@
         <v>18270.536390593461</v>
       </c>
     </row>
-    <row r="64" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -15067,6 +15255,9 @@
       <c r="BK64">
         <v>1511.6216457830969</v>
       </c>
+      <c r="BL64">
+        <v>0</v>
+      </c>
       <c r="BM64">
         <v>667.08320320631674</v>
       </c>
@@ -15107,7 +15298,7 @@
         <v>18825.58100033037</v>
       </c>
     </row>
-    <row r="65" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -15300,6 +15491,9 @@
       <c r="BL65">
         <v>667.08320320631674</v>
       </c>
+      <c r="BM65">
+        <v>0</v>
+      </c>
       <c r="BN65">
         <v>3700</v>
       </c>
@@ -15337,7 +15531,7 @@
         <v>19457.196612050771</v>
       </c>
     </row>
-    <row r="66" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -15533,6 +15727,9 @@
       <c r="BM66">
         <v>3700</v>
       </c>
+      <c r="BN66">
+        <v>0</v>
+      </c>
       <c r="BO66">
         <v>715.89105316381767</v>
       </c>
@@ -15567,7 +15764,7 @@
         <v>17809.05668473207</v>
       </c>
     </row>
-    <row r="67" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -15766,6 +15963,9 @@
       <c r="BN67">
         <v>715.89105316381767</v>
       </c>
+      <c r="BO67">
+        <v>0</v>
+      </c>
       <c r="BP67">
         <v>3707.4249823833252</v>
       </c>
@@ -15797,7 +15997,7 @@
         <v>17094.5897874152</v>
       </c>
     </row>
-    <row r="68" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -15999,6 +16199,9 @@
       <c r="BO68">
         <v>3707.4249823833252</v>
       </c>
+      <c r="BP68">
+        <v>0</v>
+      </c>
       <c r="BQ68">
         <v>1192.6860441876561</v>
       </c>
@@ -16027,7 +16230,7 @@
         <v>16787.197502859141</v>
       </c>
     </row>
-    <row r="69" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -16232,6 +16435,9 @@
       <c r="BP69">
         <v>1192.6860441876561</v>
       </c>
+      <c r="BQ69">
+        <v>0</v>
+      </c>
       <c r="BR69">
         <v>1432.6548781894401</v>
       </c>
@@ -16257,7 +16463,7 @@
         <v>16020.37764848257</v>
       </c>
     </row>
-    <row r="70" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -16465,6 +16671,9 @@
       <c r="BQ70">
         <v>1432.6548781894401</v>
       </c>
+      <c r="BR70">
+        <v>0</v>
+      </c>
       <c r="BS70">
         <v>4964.8766349225634</v>
       </c>
@@ -16487,7 +16696,7 @@
         <v>14721.75261305528</v>
       </c>
     </row>
-    <row r="71" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -16698,6 +16907,9 @@
       <c r="BR71">
         <v>4964.8766349225634</v>
       </c>
+      <c r="BS71">
+        <v>0</v>
+      </c>
       <c r="BT71">
         <v>9200</v>
       </c>
@@ -16717,7 +16929,7 @@
         <v>19600</v>
       </c>
     </row>
-    <row r="72" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -16931,6 +17143,9 @@
       <c r="BS72">
         <v>9200</v>
       </c>
+      <c r="BT72">
+        <v>0</v>
+      </c>
       <c r="BU72">
         <v>1900</v>
       </c>
@@ -16947,7 +17162,7 @@
         <v>21651.789764358971</v>
       </c>
     </row>
-    <row r="73" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -17164,6 +17379,9 @@
       <c r="BT73">
         <v>1900</v>
       </c>
+      <c r="BU73">
+        <v>0</v>
+      </c>
       <c r="BV73">
         <v>300</v>
       </c>
@@ -17177,7 +17395,7 @@
         <v>22524.87513838867</v>
       </c>
     </row>
-    <row r="74" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -17397,6 +17615,9 @@
       <c r="BU74">
         <v>300</v>
       </c>
+      <c r="BV74">
+        <v>0</v>
+      </c>
       <c r="BW74">
         <v>19600</v>
       </c>
@@ -17407,7 +17628,7 @@
         <v>22674.214429611449</v>
       </c>
     </row>
-    <row r="75" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -17630,6 +17851,9 @@
       <c r="BV75">
         <v>19600</v>
       </c>
+      <c r="BW75">
+        <v>0</v>
+      </c>
       <c r="BX75">
         <v>11100</v>
       </c>
@@ -17637,7 +17861,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="76" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -17863,11 +18087,14 @@
       <c r="BW76">
         <v>11100</v>
       </c>
+      <c r="BX76">
+        <v>0</v>
+      </c>
       <c r="BY76">
         <v>300</v>
       </c>
     </row>
-    <row r="77" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -18095,6 +18322,9 @@
       </c>
       <c r="BX77">
         <v>300</v>
+      </c>
+      <c r="BY77">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -18103,6 +18333,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010001C6622B9F754548848AD789019F80DC" ma:contentTypeVersion="0" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="9523c824c069ef90c31af9c6235fb814">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f87af33324d3c5e7cc78c986de44d02">
     <xsd:element name="properties">
@@ -18216,29 +18461,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0AB47CC-2F4B-4354-AB82-645E3A6E0128}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8D7DFD2-2019-4F6F-832B-B10005936C21}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F3DE5B1-E60C-4E60-8EA0-7E4344374C80}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F3DE5B1-E60C-4E60-8EA0-7E4344374C80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8D7DFD2-2019-4F6F-832B-B10005936C21}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0AB47CC-2F4B-4354-AB82-645E3A6E0128}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>